<commit_message>
Revisão geral e escrita de comentarios nos README.md individuais
ChuvaWAR

Realizado identação adequada ao código, remoção de código desnecessário e mudança no método de ordenação em Battlefield.php e por fim alteração na lógica utilizada durante definição de vizinhos no método conquer em BaseCountry.php.

GaloScrapper

Realizado alteração na identação e outra para se escrever todos os dados em maiúsculo na planilha, de modo a deixar uma melhor visualização e manipulação futura dos dados.
</commit_message>
<xml_diff>
--- a/webscrapping/result.xlsx
+++ b/webscrapping/result.xlsx
@@ -247,52 +247,52 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Structural elucidation of a novel pyrrolizidine alkaloid isolated from Crotalaria retusa L.</t>
+          <t>STRUCTURAL ELUCIDATION OF A NOVEL PYRROLIZIDINE ALKALOID ISOLATED FROM CROTALARIA RETUSA L.</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>Bryan Nickson Santana Pinto</t>
+          <t>BRYAN NICKSON SANTANA PINTO</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
+          <t>DEPARTAMENTO DE QUÍMICA / CENTRO DE CIÊNCIAS EXATAS E TECNOLÓGICAS / UNIVERSIDADE FEDERAL DE VIÇOSA - CAMPUS VIÇOSA</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t> Gabriella Almeida  Moura</t>
+          <t> GABRIELLA ALMEIDA  MOURA</t>
         </is>
       </c>
       <c r="G2" s="0" t="inlineStr">
         <is>
-          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
+          <t>DEPARTAMENTO DE QUÍMICA / CENTRO DE CIÊNCIAS EXATAS E TECNOLÓGICAS / UNIVERSIDADE FEDERAL DE VIÇOSA - CAMPUS VIÇOSA</t>
         </is>
       </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
-          <t> Antonio Demuner</t>
+          <t> ANTONIO DEMUNER</t>
         </is>
       </c>
       <c r="I2" s="0" t="inlineStr">
         <is>
-          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
+          <t>DEPARTAMENTO DE QUÍMICA / CENTRO DE CIÊNCIAS EXATAS E TECNOLÓGICAS / UNIVERSIDADE FEDERAL DE VIÇOSA - CAMPUS VIÇOSA</t>
         </is>
       </c>
       <c r="J2" s="0" t="inlineStr">
         <is>
-          <t> Elson Santiago Alvarenga</t>
+          <t> ELSON SANTIAGO ALVARENGA</t>
         </is>
       </c>
       <c r="K2" s="0" t="inlineStr">
         <is>
-          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
+          <t>DEPARTAMENTO DE QUÍMICA / CENTRO DE CIÊNCIAS EXATAS E TECNOLÓGICAS / UNIVERSIDADE FEDERAL DE VIÇOSA - CAMPUS VIÇOSA</t>
         </is>
       </c>
     </row>
@@ -307,17 +307,17 @@
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>Tiago   Bueno de Moraes</t>
+          <t>TIAGO   BUENO DE MORAES</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>Departamento de Química  / Instituto de Ciências Exatas  / Universidade Federal de Minas Gerais</t>
+          <t>DEPARTAMENTO DE QUÍMICA  / INSTITUTO DE CIÊNCIAS EXATAS  / UNIVERSIDADE FEDERAL DE MINAS GERAIS</t>
         </is>
       </c>
     </row>
@@ -332,37 +332,37 @@
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>Tatiana Monaretto</t>
+          <t>TATIANA MONARETTO</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>Centre national de la recherche scientifique (CNRS)</t>
+          <t>CENTRE NATIONAL DE LA RECHERCHE SCIENTIFIQUE (CNRS)</t>
         </is>
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t> Luiz Alberto Colnago</t>
+          <t> LUIZ ALBERTO COLNAGO</t>
         </is>
       </c>
       <c r="G4" s="0" t="inlineStr">
         <is>
-          <t>Empresa Brasileira de Pesquisa Agropecuária</t>
+          <t>EMPRESA BRASILEIRA DE PESQUISA AGROPECUÁRIA</t>
         </is>
       </c>
       <c r="H4" s="0" t="inlineStr">
         <is>
-          <t> Tiago   Bueno de Moraes</t>
+          <t> TIAGO   BUENO DE MORAES</t>
         </is>
       </c>
       <c r="I4" s="0" t="inlineStr">
         <is>
-          <t>Departamento de Química  / Instituto de Ciências Exatas  / Universidade Federal de Minas Gerais</t>
+          <t>DEPARTAMENTO DE QUÍMICA  / INSTITUTO DE CIÊNCIAS EXATAS  / UNIVERSIDADE FEDERAL DE MINAS GERAIS</t>
         </is>
       </c>
     </row>
@@ -372,172 +372,172 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Is NMR Sensitive Enough to Analyze Unconcentrated Wastewater? Direct, Real-time Monitoring of Ozone and UV Treated Wastewater Using Flow NMR</t>
+          <t>IS NMR SENSITIVE ENOUGH TO ANALYZE UNCONCENTRATED WASTEWATER? DIRECT, REAL-TIME MONITORING OF OZONE AND UV TREATED WASTEWATER USING FLOW NMR</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>Katelyn Downey</t>
+          <t>KATELYN DOWNEY</t>
         </is>
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Sciences / Environmental NMR Centre / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCES / ENVIRONMENTAL NMR CENTRE / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
-          <t> Bing Wu</t>
+          <t> BING WU</t>
         </is>
       </c>
       <c r="G5" s="0" t="inlineStr">
         <is>
-          <t>Environmental NMR Centre / University of Toronto</t>
+          <t>ENVIRONMENTAL NMR CENTRE / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="H5" s="0" t="inlineStr">
         <is>
-          <t> Rudraksha Majumdar</t>
+          <t> RUDRAKSHA MAJUMDAR</t>
         </is>
       </c>
       <c r="I5" s="0" t="inlineStr">
         <is>
-          <t>Synex Medical</t>
+          <t>SYNEX MEDICAL</t>
         </is>
       </c>
       <c r="J5" s="0" t="inlineStr">
         <is>
-          <t> Daniel Lysak</t>
+          <t> DANIEL LYSAK</t>
         </is>
       </c>
       <c r="K5" s="0" t="inlineStr">
         <is>
-          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+          <t>CHEMISTRY / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="L5" s="0" t="inlineStr">
         <is>
-          <t> Rajshree Ghosh Biswas</t>
+          <t> RAJSHREE GHOSH BISWAS</t>
         </is>
       </c>
       <c r="M5" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="N5" s="0" t="inlineStr">
         <is>
-          <t> Maryam  Tabatabaei-Anaraki</t>
+          <t> MARYAM  TABATABAEI-ANARAKI</t>
         </is>
       </c>
       <c r="O5" s="0" t="inlineStr">
         <is>
-          <t>Chemistry / Environmental NMR Centre / University of Toronto</t>
+          <t>CHEMISTRY / ENVIRONMENTAL NMR CENTRE / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="P5" s="0" t="inlineStr">
         <is>
-          <t> Amy Jenne</t>
+          <t> AMY JENNE</t>
         </is>
       </c>
       <c r="Q5" s="0" t="inlineStr">
         <is>
-          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+          <t>CHEMISTRY / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="R5" s="0" t="inlineStr">
         <is>
-          <t> Xiang You</t>
+          <t> XIANG YOU</t>
         </is>
       </c>
       <c r="S5" s="0" t="inlineStr">
         <is>
-          <t>Environmental NMR Centre / University of Toronto</t>
+          <t>ENVIRONMENTAL NMR CENTRE / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="T5" s="0" t="inlineStr">
         <is>
-          <t> Ronald Soong</t>
+          <t> RONALD SOONG</t>
         </is>
       </c>
       <c r="U5" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="V5" s="0" t="inlineStr">
         <is>
-          <t> Daniel Lane</t>
+          <t> DANIEL LANE</t>
         </is>
       </c>
       <c r="W5" s="0" t="inlineStr">
         <is>
-          <t>Environmental NMR Centre / University of Toronto</t>
+          <t>ENVIRONMENTAL NMR CENTRE / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="X5" s="0" t="inlineStr">
         <is>
-          <t> Paul Helm</t>
+          <t> PAUL HELM</t>
         </is>
       </c>
       <c r="Y5" s="0" t="inlineStr">
         <is>
-          <t>Environmental Monitoring &amp; Reporting Branch / Ontario Ministry of the Environment</t>
+          <t>ENVIRONMENTAL MONITORING &amp; REPORTING BRANCH / ONTARIO MINISTRY OF THE ENVIRONMENT</t>
         </is>
       </c>
       <c r="Z5" s="0" t="inlineStr">
         <is>
-          <t> Anna Codina</t>
+          <t> ANNA CODINA</t>
         </is>
       </c>
       <c r="AA5" s="0" t="inlineStr">
         <is>
-          <t>Bruker</t>
+          <t>BRUKER</t>
         </is>
       </c>
       <c r="AB5" s="0" t="inlineStr">
         <is>
-          <t> Venita Decker</t>
+          <t> VENITA DECKER</t>
         </is>
       </c>
       <c r="AC5" s="0" t="inlineStr">
         <is>
-          <t>Bruker</t>
+          <t>BRUKER</t>
         </is>
       </c>
       <c r="AD5" s="0" t="inlineStr">
         <is>
-          <t> Falko Busse</t>
+          <t> FALKO BUSSE</t>
         </is>
       </c>
       <c r="AE5" s="0" t="inlineStr">
         <is>
-          <t>Bruker</t>
+          <t>BRUKER</t>
         </is>
       </c>
       <c r="AF5" s="0" t="inlineStr">
         <is>
-          <t> Myrna Simpson</t>
+          <t> MYRNA SIMPSON</t>
         </is>
       </c>
       <c r="AG5" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Sciences / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCES / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="AH5" s="0" t="inlineStr">
         <is>
-          <t> Andre Simpson</t>
+          <t> ANDRE SIMPSON</t>
         </is>
       </c>
       <c r="AI5" s="0" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>UNIVERSITY OF TORONTO</t>
         </is>
       </c>
     </row>
@@ -552,57 +552,57 @@
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>Banny S. B. Correia</t>
+          <t>BANNY S. B. CORREIA</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>Instituto de Química de São Carlos  / Universidade de São Paulo</t>
+          <t>INSTITUTO DE QUÍMICA DE SÃO CARLOS  / UNIVERSIDADE DE SÃO PAULO</t>
         </is>
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
-          <t> Pollyana Ferreira da Silva Vianna</t>
+          <t> POLLYANA FERREIRA DA SILVA VIANNA</t>
         </is>
       </c>
       <c r="G6" s="0" t="inlineStr">
         <is>
-          <t>Instituto de Química de São Carlos  / Universidade de São Paulo</t>
+          <t>INSTITUTO DE QUÍMICA DE SÃO CARLOS  / UNIVERSIDADE DE SÃO PAULO</t>
         </is>
       </c>
       <c r="H6" s="0" t="inlineStr">
         <is>
-          <t> Caroline Ceribeli</t>
+          <t> CAROLINE CERIBELI</t>
         </is>
       </c>
       <c r="I6" s="0" t="inlineStr">
         <is>
-          <t>Instituto de Química de São Carlos/ Universidade de São Paulo</t>
+          <t>INSTITUTO DE QUÍMICA DE SÃO CARLOS/ UNIVERSIDADE DE SÃO PAULO</t>
         </is>
       </c>
       <c r="J6" s="0" t="inlineStr">
         <is>
-          <t> Luiz Alberto Colnago</t>
+          <t> LUIZ ALBERTO COLNAGO</t>
         </is>
       </c>
       <c r="K6" s="0" t="inlineStr">
         <is>
-          <t>Empresa Brasileira de Pesquisa Agropecuária</t>
+          <t>EMPRESA BRASILEIRA DE PESQUISA AGROPECUÁRIA</t>
         </is>
       </c>
       <c r="L6" s="0" t="inlineStr">
         <is>
-          <t> Daniel Cardoso</t>
+          <t> DANIEL CARDOSO</t>
         </is>
       </c>
       <c r="M6" s="0" t="inlineStr">
         <is>
-          <t>Instituto de Química de São Carlos  / Universidade de São Paulo</t>
+          <t>INSTITUTO DE QUÍMICA DE SÃO CARLOS  / UNIVERSIDADE DE SÃO PAULO</t>
         </is>
       </c>
     </row>
@@ -617,37 +617,37 @@
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>Enya Silva de Oliveira</t>
+          <t>ENYA SILVA DE OLIVEIRA</t>
         </is>
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>Institute of Chemistry/Federal University of Goiás</t>
+          <t>INSTITUTE OF CHEMISTRY/FEDERAL UNIVERSITY OF GOIÁS</t>
         </is>
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t> Luciano Morais Lião</t>
+          <t> LUCIANO MORAIS LIÃO</t>
         </is>
       </c>
       <c r="G7" s="0" t="inlineStr">
         <is>
-          <t>Institute of Chemistry/Federal University of Goiás</t>
+          <t>INSTITUTE OF CHEMISTRY/FEDERAL UNIVERSITY OF GOIÁS</t>
         </is>
       </c>
       <c r="H7" s="0" t="inlineStr">
         <is>
-          <t> Gerlon de Almeida Ribeiro Oliveira</t>
+          <t> GERLON DE ALMEIDA RIBEIRO OLIVEIRA</t>
         </is>
       </c>
       <c r="I7" s="0" t="inlineStr">
         <is>
-          <t>Institute of Chemistry/Federal University of Goiás</t>
+          <t>INSTITUTE OF CHEMISTRY/FEDERAL UNIVERSITY OF GOIÁS</t>
         </is>
       </c>
     </row>
@@ -662,27 +662,27 @@
       </c>
       <c r="C8" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>Amanda de Souza</t>
+          <t>AMANDA DE SOUZA</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal dos Vales do Jequitinhonha e Mucuri</t>
+          <t>UNIVERSIDADE FEDERAL DOS VALES DO JEQUITINHONHA E MUCURI</t>
         </is>
       </c>
       <c r="F8" s="0" t="inlineStr">
         <is>
-          <t> Rodrigo Verly</t>
+          <t> RODRIGO VERLY</t>
         </is>
       </c>
       <c r="G8" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal dos Vales do Jequitinhonha e Mucuri</t>
+          <t>UNIVERSIDADE FEDERAL DOS VALES DO JEQUITINHONHA E MUCURI</t>
         </is>
       </c>
     </row>
@@ -692,22 +692,22 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t> Filtered Nuclear Magnetic Resonance for in-vivo analysis</t>
+          <t> FILTERED NUCLEAR MAGNETIC RESONANCE FOR IN-VIVO ANALYSIS</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>Daniel Lysak</t>
+          <t>DANIEL LYSAK</t>
         </is>
       </c>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+          <t>CHEMISTRY / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="F9" s="0" t="inlineStr">
@@ -717,47 +717,47 @@
       </c>
       <c r="G9" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de São Carlos</t>
+          <t>UNIVERSIDADE FEDERAL DE SÃO CARLOS</t>
         </is>
       </c>
       <c r="H9" s="0" t="inlineStr">
         <is>
-          <t> Salvatore Mamone</t>
+          <t> SALVATORE MAMONE</t>
         </is>
       </c>
       <c r="I9" s="0" t="inlineStr">
         <is>
-          <t>Biophysical Chemistry / Max Planck Institute / Max Planck Institute for Biophysical Chemistry</t>
+          <t>BIOPHYSICAL CHEMISTRY / MAX PLANCK INSTITUTE / MAX PLANCK INSTITUTE FOR BIOPHYSICAL CHEMISTRY</t>
         </is>
       </c>
       <c r="J9" s="0" t="inlineStr">
         <is>
-          <t> Stefan Glöggler</t>
+          <t> STEFAN GLÖGGLER</t>
         </is>
       </c>
       <c r="K9" s="0" t="inlineStr">
         <is>
-          <t>Biophysical Chemistry / Max Planck Institute / Max Planck Institute for Biophysical Chemistry</t>
+          <t>BIOPHYSICAL CHEMISTRY / MAX PLANCK INSTITUTE / MAX PLANCK INSTITUTE FOR BIOPHYSICAL CHEMISTRY</t>
         </is>
       </c>
       <c r="L9" s="0" t="inlineStr">
         <is>
-          <t> Ronald Soong</t>
+          <t> RONALD SOONG</t>
         </is>
       </c>
       <c r="M9" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="N9" s="0" t="inlineStr">
         <is>
-          <t> Andre Simpson</t>
+          <t> ANDRE SIMPSON</t>
         </is>
       </c>
       <c r="O9" s="0" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>UNIVERSITY OF TORONTO</t>
         </is>
       </c>
     </row>
@@ -772,37 +772,37 @@
       </c>
       <c r="C10" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>Kennedy  Daniel  de Carvalho Santos</t>
+          <t>KENNEDY  DANIEL  DE CARVALHO SANTOS</t>
         </is>
       </c>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t> Guilherme Dal Poggetto</t>
+          <t> GUILHERME DAL POGGETTO</t>
         </is>
       </c>
       <c r="G10" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
       <c r="H10" s="0" t="inlineStr">
         <is>
-          <t> Cláudio Francisco Tormena</t>
+          <t> CLÁUDIO FRANCISCO TORMENA</t>
         </is>
       </c>
       <c r="I10" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
     </row>
@@ -817,57 +817,57 @@
       </c>
       <c r="C11" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>Gustavo  Solcia</t>
+          <t>GUSTAVO  SOLCIA</t>
         </is>
       </c>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>Universidade de São Paulo</t>
+          <t>UNIVERSIDADE DE SÃO PAULO</t>
         </is>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t> Caio de Jesus Oliveira</t>
+          <t> CAIO DE JESUS OLIVEIRA</t>
         </is>
       </c>
       <c r="G11" s="0" t="inlineStr">
         <is>
-          <t>Universidade de São Paulo</t>
+          <t>UNIVERSIDADE DE SÃO PAULO</t>
         </is>
       </c>
       <c r="H11" s="0" t="inlineStr">
         <is>
-          <t> Rafael Henrique Ferreira da Silva</t>
+          <t> RAFAEL HENRIQUE FERREIRA DA SILVA</t>
         </is>
       </c>
       <c r="I11" s="0" t="inlineStr">
         <is>
-          <t>Universidade de São Paulo</t>
+          <t>UNIVERSIDADE DE SÃO PAULO</t>
         </is>
       </c>
       <c r="J11" s="0" t="inlineStr">
         <is>
-          <t> Felipe Ferraz Derrico</t>
+          <t> FELIPE FERRAZ DERRICO</t>
         </is>
       </c>
       <c r="K11" s="0" t="inlineStr">
         <is>
-          <t>Universidade de São Paulo</t>
+          <t>UNIVERSIDADE DE SÃO PAULO</t>
         </is>
       </c>
       <c r="L11" s="0" t="inlineStr">
         <is>
-          <t> Fernando Fernandes Paiva</t>
+          <t> FERNANDO FERNANDES PAIVA</t>
         </is>
       </c>
       <c r="M11" s="0" t="inlineStr">
         <is>
-          <t>Instituto de Física de São Carlos</t>
+          <t>INSTITUTO DE FÍSICA DE SÃO CARLOS</t>
         </is>
       </c>
     </row>
@@ -882,47 +882,47 @@
       </c>
       <c r="C12" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>Pedro Henrique Soares Cardoso</t>
+          <t>PEDRO HENRIQUE SOARES CARDOSO</t>
         </is>
       </c>
       <c r="E12" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de Goiás</t>
+          <t>UNIVERSIDADE FEDERAL DE GOIÁS</t>
         </is>
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
-          <t> Luciano Morais Lião</t>
+          <t> LUCIANO MORAIS LIÃO</t>
         </is>
       </c>
       <c r="G12" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de Goiás</t>
+          <t>UNIVERSIDADE FEDERAL DE GOIÁS</t>
         </is>
       </c>
       <c r="H12" s="0" t="inlineStr">
         <is>
-          <t> Enya Silva de Oliveira</t>
+          <t> ENYA SILVA DE OLIVEIRA</t>
         </is>
       </c>
       <c r="I12" s="0" t="inlineStr">
         <is>
-          <t>Institute of Chemistry/Federal University of Goiás</t>
+          <t>INSTITUTE OF CHEMISTRY/FEDERAL UNIVERSITY OF GOIÁS</t>
         </is>
       </c>
       <c r="J12" s="0" t="inlineStr">
         <is>
-          <t> Gerlon de Almeida Ribeiro Oliveira</t>
+          <t> GERLON DE ALMEIDA RIBEIRO OLIVEIRA</t>
         </is>
       </c>
       <c r="K12" s="0" t="inlineStr">
         <is>
-          <t>Instituto de Química / Universidade Federal de Goiás</t>
+          <t>INSTITUTO DE QUÍMICA / UNIVERSIDADE FEDERAL DE GOIÁS</t>
         </is>
       </c>
     </row>
@@ -932,42 +932,42 @@
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>The degradation of sofosbuvir under acid stress: a mixture analysis approach by NMR spectroscopy</t>
+          <t>THE DEGRADATION OF SOFOSBUVIR UNDER ACID STRESS: A MIXTURE ANALYSIS APPROACH BY NMR SPECTROSCOPY</t>
         </is>
       </c>
       <c r="C13" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>Marília Vilela Salvador</t>
+          <t>MARÍLIA VILELA SALVADOR</t>
         </is>
       </c>
       <c r="E13" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Rio Grande do Sul</t>
+          <t>UNIVERSIDADE FEDERAL DO RIO GRANDE DO SUL</t>
         </is>
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t> Tiago  Venâncio</t>
+          <t> TIAGO  VENÂNCIO</t>
         </is>
       </c>
       <c r="G13" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de São Carlos</t>
+          <t>UNIVERSIDADE FEDERAL DE SÃO CARLOS</t>
         </is>
       </c>
       <c r="H13" s="0" t="inlineStr">
         <is>
-          <t> Francisco Paulo dos Santos</t>
+          <t> FRANCISCO PAULO DOS SANTOS</t>
         </is>
       </c>
       <c r="I13" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Rio Grande do Sul</t>
+          <t>UNIVERSIDADE FEDERAL DO RIO GRANDE DO SUL</t>
         </is>
       </c>
     </row>
@@ -982,97 +982,97 @@
       </c>
       <c r="C14" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>Monica Bastawrous</t>
+          <t>MONICA BASTAWROUS</t>
         </is>
       </c>
       <c r="E14" s="0" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="F14" s="0" t="inlineStr">
         <is>
-          <t> Rajshree Ghosh Biswas</t>
+          <t> RAJSHREE GHOSH BISWAS</t>
         </is>
       </c>
       <c r="G14" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="H14" s="0" t="inlineStr">
         <is>
-          <t> Ronald Soong</t>
+          <t> RONALD SOONG</t>
         </is>
       </c>
       <c r="I14" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="J14" s="0" t="inlineStr">
         <is>
-          <t> Sagar Wadhwa</t>
+          <t> SAGAR WADHWA</t>
         </is>
       </c>
       <c r="K14" s="0" t="inlineStr">
         <is>
-          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+          <t>INSTITUTE OF MICROSTRUCTURE TECHNOLOGY / KARLSRUHE INSTITUTE OF TECHNOLOGY / KARLSRUHE INSTITUTE OF TECHNOLOGY</t>
         </is>
       </c>
       <c r="L14" s="0" t="inlineStr">
         <is>
-          <t> Neil Mackinnon</t>
+          <t> NEIL MACKINNON</t>
         </is>
       </c>
       <c r="M14" s="0" t="inlineStr">
         <is>
-          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+          <t>INSTITUTE OF MICROSTRUCTURE TECHNOLOGY / KARLSRUHE INSTITUTE OF TECHNOLOGY / KARLSRUHE INSTITUTE OF TECHNOLOGY</t>
         </is>
       </c>
       <c r="N14" s="0" t="inlineStr">
         <is>
-          <t> Mazin Jouda</t>
+          <t> MAZIN JOUDA</t>
         </is>
       </c>
       <c r="O14" s="0" t="inlineStr">
         <is>
-          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+          <t>INSTITUTE OF MICROSTRUCTURE TECHNOLOGY / KARLSRUHE INSTITUTE OF TECHNOLOGY / KARLSRUHE INSTITUTE OF TECHNOLOGY</t>
         </is>
       </c>
       <c r="P14" s="0" t="inlineStr">
         <is>
-          <t> Dario Mager</t>
+          <t> DARIO MAGER</t>
         </is>
       </c>
       <c r="Q14" s="0" t="inlineStr">
         <is>
-          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+          <t>INSTITUTE OF MICROSTRUCTURE TECHNOLOGY / KARLSRUHE INSTITUTE OF TECHNOLOGY / KARLSRUHE INSTITUTE OF TECHNOLOGY</t>
         </is>
       </c>
       <c r="R14" s="0" t="inlineStr">
         <is>
-          <t> Jan Korvink</t>
+          <t> JAN KORVINK</t>
         </is>
       </c>
       <c r="S14" s="0" t="inlineStr">
         <is>
-          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+          <t>INSTITUTE OF MICROSTRUCTURE TECHNOLOGY / KARLSRUHE INSTITUTE OF TECHNOLOGY / KARLSRUHE INSTITUTE OF TECHNOLOGY</t>
         </is>
       </c>
       <c r="T14" s="0" t="inlineStr">
         <is>
-          <t> Andre Simpson</t>
+          <t> ANDRE SIMPSON</t>
         </is>
       </c>
       <c r="U14" s="0" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>UNIVERSITY OF TORONTO</t>
         </is>
       </c>
     </row>
@@ -1082,92 +1082,92 @@
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>Inhibition of β-lactamases OXA-143 by hydrolyzed meropenem</t>
+          <t>INHIBITION OF Β-LACTAMASES OXA-143 BY HYDROLYZED MEROPENEM</t>
         </is>
       </c>
       <c r="C15" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>Yara Rocha</t>
+          <t>YARA ROCHA</t>
         </is>
       </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t> Victor U. Antunes</t>
+          <t> VICTOR U. ANTUNES</t>
         </is>
       </c>
       <c r="G15" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
       <c r="H15" s="0" t="inlineStr">
         <is>
-          <t> Yan  Ladeira</t>
+          <t> YAN  LADEIRA</t>
         </is>
       </c>
       <c r="I15" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de Minas Gerais</t>
+          <t>UNIVERSIDADE FEDERAL DE MINAS GERAIS</t>
         </is>
       </c>
       <c r="J15" s="0" t="inlineStr">
         <is>
-          <t> Adolfo Henrique de Moraes Silva</t>
+          <t> ADOLFO HENRIQUE DE MORAES SILVA</t>
         </is>
       </c>
       <c r="K15" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de Minas Gerais</t>
+          <t>UNIVERSIDADE FEDERAL DE MINAS GERAIS</t>
         </is>
       </c>
       <c r="L15" s="0" t="inlineStr">
         <is>
-          <t> Renan Pirolla</t>
+          <t> RENAN PIROLLA</t>
         </is>
       </c>
       <c r="M15" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
       <c r="N15" s="0" t="inlineStr">
         <is>
-          <t> Fábio Gozzo</t>
+          <t> FÁBIO GOZZO</t>
         </is>
       </c>
       <c r="O15" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
       <c r="P15" s="0" t="inlineStr">
         <is>
-          <t> Anthony  Mittermaier</t>
+          <t> ANTHONY  MITTERMAIER</t>
         </is>
       </c>
       <c r="Q15" s="0" t="inlineStr">
         <is>
-          <t>Department of Chemistry / McGill University / McGill University</t>
+          <t>DEPARTMENT OF CHEMISTRY / MCGILL UNIVERSITY / MCGILL UNIVERSITY</t>
         </is>
       </c>
       <c r="R15" s="0" t="inlineStr">
         <is>
-          <t> Denize  C. Favaro</t>
+          <t> DENIZE  C. FAVARO</t>
         </is>
       </c>
       <c r="S15" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
     </row>
@@ -1177,32 +1177,32 @@
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>Evaluation of intramolecular hydrogen bonding on fluorinated pyridines   </t>
+          <t>EVALUATION OF INTRAMOLECULAR HYDROGEN BONDING ON FLUORINATED PYRIDINES   </t>
         </is>
       </c>
       <c r="C16" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>Cassia  Chiari</t>
+          <t>CASSIA  CHIARI</t>
         </is>
       </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
       <c r="F16" s="0" t="inlineStr">
         <is>
-          <t> Cláudio Francisco Tormena</t>
+          <t> CLÁUDIO FRANCISCO TORMENA</t>
         </is>
       </c>
       <c r="G16" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
     </row>
@@ -1217,37 +1217,37 @@
       </c>
       <c r="C17" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>Flávio Bueno dos Santos</t>
+          <t>FLÁVIO BUENO DOS SANTOS</t>
         </is>
       </c>
       <c r="E17" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de Ouro Preto</t>
+          <t>UNIVERSIDADE FEDERAL DE OURO PRETO</t>
         </is>
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t> Marcus Cardoso</t>
+          <t> MARCUS CARDOSO</t>
         </is>
       </c>
       <c r="G17" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de Ouro Preto</t>
+          <t>UNIVERSIDADE FEDERAL DE OURO PRETO</t>
         </is>
       </c>
       <c r="H17" s="0" t="inlineStr">
         <is>
-          <t> Jose Rivera</t>
+          <t> JOSE RIVERA</t>
         </is>
       </c>
       <c r="I17" s="0" t="inlineStr">
         <is>
-          <t>Universidade de São Paulo</t>
+          <t>UNIVERSIDADE DE SÃO PAULO</t>
         </is>
       </c>
     </row>
@@ -1257,72 +1257,72 @@
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>DIRECT qNMR MEASUREMENTS</t>
+          <t>DIRECT QNMR MEASUREMENTS</t>
         </is>
       </c>
       <c r="C18" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>Priscila  Rubim</t>
+          <t>PRISCILA  RUBIM</t>
         </is>
       </c>
       <c r="E18" s="0" t="inlineStr">
         <is>
-          <t>Instituto Militar de Engenharia</t>
+          <t>INSTITUTO MILITAR DE ENGENHARIA</t>
         </is>
       </c>
       <c r="F18" s="0" t="inlineStr">
         <is>
-          <t> Mychelle Monteiro</t>
+          <t> MYCHELLE MONTEIRO</t>
         </is>
       </c>
       <c r="G18" s="0" t="inlineStr">
         <is>
-          <t>INCQS / Fundação Oswaldo Cruz</t>
+          <t>INCQS / FUNDAÇÃO OSWALDO CRUZ</t>
         </is>
       </c>
       <c r="H18" s="0" t="inlineStr">
         <is>
-          <t> Filipe Soares Quirino da Silva</t>
+          <t> FILIPE SOARES QUIRINO DA SILVA</t>
         </is>
       </c>
       <c r="I18" s="0" t="inlineStr">
         <is>
-          <t>INCQS/Fiocruz</t>
+          <t>INCQS/FIOCRUZ</t>
         </is>
       </c>
       <c r="J18" s="0" t="inlineStr">
         <is>
-          <t> Tanos Celmar Costa França</t>
+          <t> TANOS CELMAR COSTA FRANÇA</t>
         </is>
       </c>
       <c r="K18" s="0" t="inlineStr">
         <is>
-          <t>Instituto Militar de Engenharia</t>
+          <t>INSTITUTO MILITAR DE ENGENHARIA</t>
         </is>
       </c>
       <c r="L18" s="0" t="inlineStr">
         <is>
-          <t> Joyce Sobreiro Francisco Diz de Almeida</t>
+          <t> JOYCE SOBREIRO FRANCISCO DIZ DE ALMEIDA</t>
         </is>
       </c>
       <c r="M18" s="0" t="inlineStr">
         <is>
-          <t>Instituto Militar de Engenharia</t>
+          <t>INSTITUTO MILITAR DE ENGENHARIA</t>
         </is>
       </c>
       <c r="N18" s="0" t="inlineStr">
         <is>
-          <t> Jochen  Junker</t>
+          <t> JOCHEN  JUNKER</t>
         </is>
       </c>
       <c r="O18" s="0" t="inlineStr">
         <is>
-          <t>CDTS / Presidência / Fundação Oswaldo Cruz</t>
+          <t>CDTS / PRESIDÊNCIA / FUNDAÇÃO OSWALDO CRUZ</t>
         </is>
       </c>
     </row>
@@ -1337,27 +1337,27 @@
       </c>
       <c r="C19" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>Laiza  Bruzadelle Loureiro</t>
+          <t>LAIZA  BRUZADELLE LOUREIRO</t>
         </is>
       </c>
       <c r="E19" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t> Cláudio Francisco Tormena</t>
+          <t> CLÁUDIO FRANCISCO TORMENA</t>
         </is>
       </c>
       <c r="G19" s="0" t="inlineStr">
         <is>
-          <t>Universidade Estadual de Campinas</t>
+          <t>UNIVERSIDADE ESTADUAL DE CAMPINAS</t>
         </is>
       </c>
     </row>
@@ -1367,52 +1367,52 @@
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>qNMR APPROACH FOR MONITORING CHANGES IN CARANHA FISH POLAR AND NON-POLAR METABOLIC PROFILES DUE TO FREEZE-THAW CYCLES</t>
+          <t>QNMR APPROACH FOR MONITORING CHANGES IN CARANHA FISH POLAR AND NON-POLAR METABOLIC PROFILES DUE TO FREEZE-THAW CYCLES</t>
         </is>
       </c>
       <c r="C20" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>Vinícius  Silva Pinto</t>
+          <t>VINÍCIUS  SILVA PINTO</t>
         </is>
       </c>
       <c r="E20" s="0" t="inlineStr">
         <is>
-          <t>Federal Institute Goiano</t>
+          <t>FEDERAL INSTITUTE GOIANO</t>
         </is>
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
-          <t> Christian Dias Gomides</t>
+          <t> CHRISTIAN DIAS GOMIDES</t>
         </is>
       </c>
       <c r="G20" s="0" t="inlineStr">
         <is>
-          <t>Institute of Chemistry, Federal University of Goias</t>
+          <t>INSTITUTE OF CHEMISTRY, FEDERAL UNIVERSITY OF GOIAS</t>
         </is>
       </c>
       <c r="H20" s="0" t="inlineStr">
         <is>
-          <t> Igor Flores</t>
+          <t> IGOR FLORES</t>
         </is>
       </c>
       <c r="I20" s="0" t="inlineStr">
         <is>
-          <t>Federal Institute of Goiás</t>
+          <t>FEDERAL INSTITUTE OF GOIÁS</t>
         </is>
       </c>
       <c r="J20" s="0" t="inlineStr">
         <is>
-          <t> Luciano Morais Lião</t>
+          <t> LUCIANO MORAIS LIÃO</t>
         </is>
       </c>
       <c r="K20" s="0" t="inlineStr">
         <is>
-          <t>Institute of Chemistry, Federal University of Goias</t>
+          <t>INSTITUTE OF CHEMISTRY, FEDERAL UNIVERSITY OF GOIAS</t>
         </is>
       </c>
     </row>
@@ -1427,47 +1427,47 @@
       </c>
       <c r="C21" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>José Dias de Souza Filho</t>
+          <t>JOSÉ DIAS DE SOUZA FILHO</t>
         </is>
       </c>
       <c r="E21" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de Ouro Preto</t>
+          <t>UNIVERSIDADE FEDERAL DE OURO PRETO</t>
         </is>
       </c>
       <c r="F21" s="0" t="inlineStr">
         <is>
-          <t> Jacqueline Souza</t>
+          <t> JACQUELINE SOUZA</t>
         </is>
       </c>
       <c r="G21" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de Ouro Preto</t>
+          <t>UNIVERSIDADE FEDERAL DE OURO PRETO</t>
         </is>
       </c>
       <c r="H21" s="0" t="inlineStr">
         <is>
-          <t> Marta de Lana</t>
+          <t> MARTA DE LANA</t>
         </is>
       </c>
       <c r="I21" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de Ouro Preto</t>
+          <t>UNIVERSIDADE FEDERAL DE OURO PRETO</t>
         </is>
       </c>
       <c r="J21" s="0" t="inlineStr">
         <is>
-          <t> Gabriela Roberta Ramos Fernandes</t>
+          <t> GABRIELA ROBERTA RAMOS FERNANDES</t>
         </is>
       </c>
       <c r="K21" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de Ouro Preto</t>
+          <t>UNIVERSIDADE FEDERAL DE OURO PRETO</t>
         </is>
       </c>
     </row>
@@ -1482,57 +1482,57 @@
       </c>
       <c r="C22" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>Beatriz Rosa  Penna</t>
+          <t>BEATRIZ ROSA  PENNA</t>
         </is>
       </c>
       <c r="E22" s="0" t="inlineStr">
         <is>
-          <t>Instituto de Bioquímica Médica, Centro Nacional de Ressonância Magnética Nuclear Jiri Jonas, Universidade Federal do Rio de Janeiro</t>
+          <t>INSTITUTO DE BIOQUÍMICA MÉDICA, CENTRO NACIONAL DE RESSONÂNCIA MAGNÉTICA NUCLEAR JIRI JONAS, UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="F22" s="0" t="inlineStr">
         <is>
-          <t> Thamires Moreira</t>
+          <t> THAMIRES MOREIRA</t>
         </is>
       </c>
       <c r="G22" s="0" t="inlineStr">
         <is>
-          <t>Departamento de Bioquímica, Instituto de Química, Universidade Federal do Rio de Janeiro</t>
+          <t>DEPARTAMENTO DE BIOQUÍMICA, INSTITUTO DE QUÍMICA, UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="H22" s="0" t="inlineStr">
         <is>
-          <t> Danielle Maria  Perpétua de Oliveira Santos</t>
+          <t> DANIELLE MARIA  PERPÉTUA DE OLIVEIRA SANTOS</t>
         </is>
       </c>
       <c r="I22" s="0" t="inlineStr">
         <is>
-          <t>Departamento de Bioquímica, Instituto de Química, Universidade Federal do Rio de Janeiro</t>
+          <t>DEPARTAMENTO DE BIOQUÍMICA, INSTITUTO DE QUÍMICA, UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="J22" s="0" t="inlineStr">
         <is>
-          <t> Cristiane Dinis Ano Bom</t>
+          <t> CRISTIANE DINIS ANO BOM</t>
         </is>
       </c>
       <c r="K22" s="0" t="inlineStr">
         <is>
-          <t>Departamento de Bioquímica, Instituto de Química, Universidade Federal do Rio de Janeiro</t>
+          <t>DEPARTAMENTO DE BIOQUÍMICA, INSTITUTO DE QUÍMICA, UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="L22" s="0" t="inlineStr">
         <is>
-          <t> Ana Paula Valente</t>
+          <t> ANA PAULA VALENTE</t>
         </is>
       </c>
       <c r="M22" s="0" t="inlineStr">
         <is>
-          <t>Instituto de Bioquímica Médica, Centro Nacional de Ressonância Magnética Nuclear Jiri Jonas, Universidade Federal do Rio de Janeiro</t>
+          <t>INSTITUTO DE BIOQUÍMICA MÉDICA, CENTRO NACIONAL DE RESSONÂNCIA MAGNÉTICA NUCLEAR JIRI JONAS, UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
     </row>
@@ -1547,77 +1547,77 @@
       </c>
       <c r="C23" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>Julie Lopes</t>
+          <t>JULIE LOPES</t>
         </is>
       </c>
       <c r="E23" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Rio de Janeiro</t>
+          <t>UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
-          <t> Beatriz Rosa  Penna</t>
+          <t> BEATRIZ ROSA  PENNA</t>
         </is>
       </c>
       <c r="G23" s="0" t="inlineStr">
         <is>
-          <t>Instituto de Bioquímica Médica, Centro Nacional de Ressonância Magnética Nuclear Jiri Jonas, Universidade Federal do Rio de Janeiro</t>
+          <t>INSTITUTO DE BIOQUÍMICA MÉDICA, CENTRO NACIONAL DE RESSONÂNCIA MAGNÉTICA NUCLEAR JIRI JONAS, UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="H23" s="0" t="inlineStr">
         <is>
-          <t> Ana Paula Valente</t>
+          <t> ANA PAULA VALENTE</t>
         </is>
       </c>
       <c r="I23" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Rio de Janeiro</t>
+          <t>UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="J23" s="0" t="inlineStr">
         <is>
-          <t> Leonardo  Bartkevihi</t>
+          <t> LEONARDO  BARTKEVIHI</t>
         </is>
       </c>
       <c r="K23" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Rio de Janeiro</t>
+          <t>UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="L23" s="0" t="inlineStr">
         <is>
-          <t> Paulo Antônio de Souza Mourão</t>
+          <t> PAULO ANTÔNIO DE SOUZA MOURÃO</t>
         </is>
       </c>
       <c r="M23" s="0" t="inlineStr">
         <is>
-          <t>Laboratório de Tecido Conjuntivo / Instituto de Bioquímica Médica / Universidade Federal de Juiz de Fora</t>
+          <t>LABORATÓRIO DE TECIDO CONJUNTIVO / INSTITUTO DE BIOQUÍMICA MÉDICA / UNIVERSIDADE FEDERAL DE JUIZ DE FORA</t>
         </is>
       </c>
       <c r="N23" s="0" t="inlineStr">
         <is>
-          <t> Francisco  Felipe  Bezerra</t>
+          <t> FRANCISCO  FELIPE  BEZERRA</t>
         </is>
       </c>
       <c r="O23" s="0" t="inlineStr">
         <is>
-          <t>Departamento de Glicobiologia  / Bioquímica Médica / Universidade Federal do Rio de Janeiro</t>
+          <t>DEPARTAMENTO DE GLICOBIOLOGIA  / BIOQUÍMICA MÉDICA / UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="P23" s="0" t="inlineStr">
         <is>
-          <t> Adriane Regina Todeschini</t>
+          <t> ADRIANE REGINA TODESCHINI</t>
         </is>
       </c>
       <c r="Q23" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Rio de Janeiro</t>
+          <t>UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
     </row>
@@ -1632,47 +1632,47 @@
       </c>
       <c r="C24" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>Elton Tadeu Montrazi</t>
+          <t>ELTON TADEU MONTRAZI</t>
         </is>
       </c>
       <c r="E24" s="0" t="inlineStr">
         <is>
-          <t>Department of Chemical and Biological Physics, Weizmann Institute of Science, Israel</t>
+          <t>DEPARTMENT OF CHEMICAL AND BIOLOGICAL PHYSICS, WEIZMANN INSTITUTE OF SCIENCE, ISRAEL</t>
         </is>
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
-          <t> Tatiana Monaretto</t>
+          <t> TATIANA MONARETTO</t>
         </is>
       </c>
       <c r="G24" s="0" t="inlineStr">
         <is>
-          <t>Centre National de La Recherche Scientifique, France</t>
+          <t>CENTRE NATIONAL DE LA RECHERCHE SCIENTIFIQUE, FRANCE</t>
         </is>
       </c>
       <c r="H24" s="0" t="inlineStr">
         <is>
-          <t> Luiz Alberto Colnago</t>
+          <t> LUIZ ALBERTO COLNAGO</t>
         </is>
       </c>
       <c r="I24" s="0" t="inlineStr">
         <is>
-          <t>Embrapa Instrumentation, Brazil</t>
+          <t>EMBRAPA INSTRUMENTATION, BRAZIL</t>
         </is>
       </c>
       <c r="J24" s="0" t="inlineStr">
         <is>
-          <t> Tito José Bonagamba</t>
+          <t> TITO JOSÉ BONAGAMBA</t>
         </is>
       </c>
       <c r="K24" s="0" t="inlineStr">
         <is>
-          <t>São Carlos Institute of Physics, University of São Paulo, Brazil</t>
+          <t>SÃO CARLOS INSTITUTE OF PHYSICS, UNIVERSITY OF SÃO PAULO, BRAZIL</t>
         </is>
       </c>
     </row>
@@ -1687,17 +1687,17 @@
       </c>
       <c r="C25" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>Tatiana Monaretto</t>
+          <t>TATIANA MONARETTO</t>
         </is>
       </c>
       <c r="E25" s="0" t="inlineStr">
         <is>
-          <t>Centre national de la recherche scientifique (CNRS)</t>
+          <t>CENTRE NATIONAL DE LA RECHERCHE SCIENTIFIQUE (CNRS)</t>
         </is>
       </c>
     </row>
@@ -1712,17 +1712,17 @@
       </c>
       <c r="C26" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>Patrick Giraudeau</t>
+          <t>PATRICK GIRAUDEAU</t>
         </is>
       </c>
       <c r="E26" s="0" t="inlineStr">
         <is>
-          <t>CEISAM / Faculté des Sciences et Techniques / Université de Nantes</t>
+          <t>CEISAM / FACULTÉ DES SCIENCES ET TECHNIQUES / UNIVERSITÉ DE NANTES</t>
         </is>
       </c>
     </row>
@@ -1737,17 +1737,17 @@
       </c>
       <c r="C27" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>Andre Simpson</t>
+          <t>ANDRE SIMPSON</t>
         </is>
       </c>
       <c r="E27" s="0" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>UNIVERSITY OF TORONTO</t>
         </is>
       </c>
     </row>
@@ -1757,22 +1757,22 @@
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>Intelligent TD NMR Relaxation Sensor for Monitoring of PUFA-rich Food Products Oxidation</t>
+          <t>INTELLIGENT TD NMR RELAXATION SENSOR FOR MONITORING OF PUFA-RICH FOOD PRODUCTS OXIDATION</t>
         </is>
       </c>
       <c r="C28" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>Zeev Wiesman</t>
+          <t>ZEEV WIESMAN</t>
         </is>
       </c>
       <c r="E28" s="0" t="inlineStr">
         <is>
-          <t>LowField</t>
+          <t>LOWFIELD</t>
         </is>
       </c>
     </row>
@@ -1782,32 +1782,32 @@
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>NMR applied to investigate coordination compounds towards biological challenges</t>
+          <t>NMR APPLIED TO INVESTIGATE COORDINATION COMPOUNDS TOWARDS BIOLOGICAL CHALLENGES</t>
         </is>
       </c>
       <c r="C29" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>Flavio Vinicius Crizostomo  Kock</t>
+          <t>FLAVIO VINICIUS CRIZOSTOMO  KOCK</t>
         </is>
       </c>
       <c r="E29" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de São Carlos</t>
+          <t>UNIVERSIDADE FEDERAL DE SÃO CARLOS</t>
         </is>
       </c>
       <c r="F29" s="0" t="inlineStr">
         <is>
-          <t> Tiago Venâncio</t>
+          <t> TIAGO VENÂNCIO</t>
         </is>
       </c>
       <c r="G29" s="0" t="inlineStr">
         <is>
-          <t>Departamento de Química / Universidade Federal de São Carlos</t>
+          <t>DEPARTAMENTO DE QUÍMICA / UNIVERSIDADE FEDERAL DE SÃO CARLOS</t>
         </is>
       </c>
     </row>
@@ -1822,17 +1822,17 @@
       </c>
       <c r="C30" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>Juan Miguel López del Amo</t>
+          <t>JUAN MIGUEL LÓPEZ DEL AMO</t>
         </is>
       </c>
       <c r="E30" s="0" t="inlineStr">
         <is>
-          <t>NMR  / CIC energigune / CIC energigune</t>
+          <t>NMR  / CIC ENERGIGUNE / CIC ENERGIGUNE</t>
         </is>
       </c>
     </row>
@@ -1847,17 +1847,17 @@
       </c>
       <c r="C31" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>Jeffrey Reimer</t>
+          <t>JEFFREY REIMER</t>
         </is>
       </c>
       <c r="E31" s="0" t="inlineStr">
         <is>
-          <t>Dept Chem and BioM Engr / University of California</t>
+          <t>DEPT CHEM AND BIOM ENGR / UNIVERSITY OF CALIFORNIA</t>
         </is>
       </c>
     </row>
@@ -1872,17 +1872,17 @@
       </c>
       <c r="C32" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D32" s="0" t="inlineStr">
         <is>
-          <t>Daniel Huster</t>
+          <t>DANIEL HUSTER</t>
         </is>
       </c>
       <c r="E32" s="0" t="inlineStr">
         <is>
-          <t>University of Leipzig</t>
+          <t>UNIVERSITY OF LEIPZIG</t>
         </is>
       </c>
     </row>
@@ -1897,17 +1897,17 @@
       </c>
       <c r="C33" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D33" s="0" t="inlineStr">
         <is>
-          <t>Pau Nolis</t>
+          <t>PAU NOLIS</t>
         </is>
       </c>
       <c r="E33" s="0" t="inlineStr">
         <is>
-          <t>Universitat Autònoma de Barcelona</t>
+          <t>UNIVERSITAT AUTÒNOMA DE BARCELONA</t>
         </is>
       </c>
     </row>
@@ -1917,22 +1917,22 @@
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
-          <t>Advanced NMR Methods to Solve Complex Molecular Structures</t>
+          <t>ADVANCED NMR METHODS TO SOLVE COMPLEX MOLECULAR STRUCTURES</t>
         </is>
       </c>
       <c r="C34" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D34" s="0" t="inlineStr">
         <is>
-          <t>Josep Saurí</t>
+          <t>JOSEP SAURÍ</t>
         </is>
       </c>
       <c r="E34" s="0" t="inlineStr">
         <is>
-          <t>NMR Research Scientist</t>
+          <t>NMR RESEARCH SCIENTIST</t>
         </is>
       </c>
     </row>
@@ -1942,22 +1942,22 @@
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
-          <t>Recent Selective Excitation Methods for the Investigation of Molecular Structure</t>
+          <t>RECENT SELECTIVE EXCITATION METHODS FOR THE INVESTIGATION OF MOLECULAR STRUCTURE</t>
         </is>
       </c>
       <c r="C35" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D35" s="0" t="inlineStr">
         <is>
-          <t>Gareth Morris</t>
+          <t>GARETH MORRIS</t>
         </is>
       </c>
       <c r="E35" s="0" t="inlineStr">
         <is>
-          <t>The University of Manchester</t>
+          <t>THE UNIVERSITY OF MANCHESTER</t>
         </is>
       </c>
     </row>
@@ -1967,22 +1967,22 @@
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
-          <t>Prospecting of chemical residues generated by orange processing using the NMR technique – an overview</t>
+          <t>PROSPECTING OF CHEMICAL RESIDUES GENERATED BY ORANGE PROCESSING USING THE NMR TECHNIQUE – AN OVERVIEW</t>
         </is>
       </c>
       <c r="C36" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D36" s="0" t="inlineStr">
         <is>
-          <t>Antonio Gilberto Ferreira</t>
+          <t>ANTONIO GILBERTO FERREIRA</t>
         </is>
       </c>
       <c r="E36" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de São Carlos</t>
+          <t>UNIVERSIDADE FEDERAL DE SÃO CARLOS</t>
         </is>
       </c>
     </row>
@@ -1992,22 +1992,22 @@
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
-          <t>The Role of Water Scaffolds in Regulating Enzyme Structure &amp; Dynamics</t>
+          <t>THE ROLE OF WATER SCAFFOLDS IN REGULATING ENZYME STRUCTURE &amp; DYNAMICS</t>
         </is>
       </c>
       <c r="C37" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D37" s="0" t="inlineStr">
         <is>
-          <t>Scott Prosser</t>
+          <t>SCOTT PROSSER</t>
         </is>
       </c>
       <c r="E37" s="0" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>UNIVERSITY OF TORONTO</t>
         </is>
       </c>
     </row>
@@ -2017,42 +2017,42 @@
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
-          <t>A new method to measure the temporal magnetic field instabilities in cryogen-free magnets for magnetic resonance </t>
+          <t>A NEW METHOD TO MEASURE THE TEMPORAL MAGNETIC FIELD INSTABILITIES IN CRYOGEN-FREE MAGNETS FOR MAGNETIC RESONANCE </t>
         </is>
       </c>
       <c r="C38" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D38" s="0" t="inlineStr">
         <is>
-          <t> Jeremy Good</t>
+          <t> JEREMY GOOD</t>
         </is>
       </c>
       <c r="E38" s="0" t="inlineStr">
         <is>
-          <t>London, UK / Cryogenic Ltd</t>
+          <t>LONDON, UK / CRYOGENIC LTD</t>
         </is>
       </c>
       <c r="F38" s="0" t="inlineStr">
         <is>
-          <t> Eugeny Kryukov</t>
+          <t> EUGENY KRYUKOV</t>
         </is>
       </c>
       <c r="G38" s="0" t="inlineStr">
         <is>
-          <t>Cryogenic Ltd</t>
+          <t>CRYOGENIC LTD</t>
         </is>
       </c>
       <c r="H38" s="0" t="inlineStr">
         <is>
-          <t> Dr. Stephen Burgess</t>
+          <t> DR. STEPHEN BURGESS</t>
         </is>
       </c>
       <c r="I38" s="0" t="inlineStr">
         <is>
-          <t>Cryogenic Ltd</t>
+          <t>CRYOGENIC LTD</t>
         </is>
       </c>
     </row>
@@ -2067,17 +2067,17 @@
       </c>
       <c r="C39" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D39" s="0" t="inlineStr">
         <is>
-          <t>Giselle de Araujo Lima e Souza</t>
+          <t>GISELLE DE ARAUJO LIMA E SOUZA</t>
         </is>
       </c>
       <c r="E39" s="0" t="inlineStr">
         <is>
-          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
+          <t>DEPARTMENT OF CHEMISTRY, MATERIALS AND CHEMICAL ENGINEERING “GIULIO NATTA” / POLITECNICO DI MILANO</t>
         </is>
       </c>
     </row>
@@ -2092,17 +2092,17 @@
       </c>
       <c r="C40" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D40" s="0" t="inlineStr">
         <is>
-          <t>Ariel Sarotti</t>
+          <t>ARIEL SAROTTI</t>
         </is>
       </c>
       <c r="E40" s="0" t="inlineStr">
         <is>
-          <t>Chimica / Chimica / Universidad Nacional de Rosario</t>
+          <t>CHIMICA / CHIMICA / UNIVERSIDAD NACIONAL DE ROSARIO</t>
         </is>
       </c>
     </row>
@@ -2117,27 +2117,27 @@
       </c>
       <c r="C41" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D41" s="0" t="inlineStr">
         <is>
-          <t>Sophia Hayes</t>
+          <t>SOPHIA HAYES</t>
         </is>
       </c>
       <c r="E41" s="0" t="inlineStr">
         <is>
-          <t>Chemistry / Arts &amp; Sciences / Washington University in St. Louis</t>
+          <t>CHEMISTRY / ARTS &amp; SCIENCES / WASHINGTON UNIVERSITY IN ST. LOUIS</t>
         </is>
       </c>
       <c r="F41" s="0" t="inlineStr">
         <is>
-          <t> He Sun</t>
+          <t> HE SUN</t>
         </is>
       </c>
       <c r="G41" s="0" t="inlineStr">
         <is>
-          <t>Chemistry / Arts &amp; Sciences / Washington University in St. Louis</t>
+          <t>CHEMISTRY / ARTS &amp; SCIENCES / WASHINGTON UNIVERSITY IN ST. LOUIS</t>
         </is>
       </c>
     </row>
@@ -2152,17 +2152,17 @@
       </c>
       <c r="C42" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D42" s="0" t="inlineStr">
         <is>
-          <t>Jair Freitas</t>
+          <t>JAIR FREITAS</t>
         </is>
       </c>
       <c r="E42" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Espírito Santo, Brazil</t>
+          <t>UNIVERSIDADE FEDERAL DO ESPÍRITO SANTO, BRAZIL</t>
         </is>
       </c>
     </row>
@@ -2177,17 +2177,17 @@
       </c>
       <c r="C43" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D43" s="0" t="inlineStr">
         <is>
-          <t>Toshikazu Miyoshi</t>
+          <t>TOSHIKAZU MIYOSHI</t>
         </is>
       </c>
       <c r="E43" s="0" t="inlineStr">
         <is>
-          <t>The University of Akron</t>
+          <t>THE UNIVERSITY OF AKRON</t>
         </is>
       </c>
     </row>
@@ -2202,17 +2202,17 @@
       </c>
       <c r="C44" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D44" s="0" t="inlineStr">
         <is>
-          <t>Marek Pruski</t>
+          <t>MAREK PRUSKI</t>
         </is>
       </c>
       <c r="E44" s="0" t="inlineStr">
         <is>
-          <t>Iowa State University</t>
+          <t>IOWA STATE UNIVERSITY</t>
         </is>
       </c>
     </row>
@@ -2222,22 +2222,22 @@
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
-          <t>Niumag LF-NMR/MRI application introduction</t>
+          <t>NIUMAG LF-NMR/MRI APPLICATION INTRODUCTION</t>
         </is>
       </c>
       <c r="C45" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D45" s="0" t="inlineStr">
         <is>
-          <t>Yushan Wei</t>
+          <t>YUSHAN WEI</t>
         </is>
       </c>
       <c r="E45" s="0" t="inlineStr">
         <is>
-          <t>Niumag</t>
+          <t>NIUMAG</t>
         </is>
       </c>
     </row>
@@ -2252,17 +2252,17 @@
       </c>
       <c r="C46" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D46" s="0" t="inlineStr">
         <is>
-          <t>Juan Araneda</t>
+          <t>JUAN ARANEDA</t>
         </is>
       </c>
       <c r="E46" s="0" t="inlineStr">
         <is>
-          <t>Nanalysis Corp.</t>
+          <t>NANALYSIS CORP.</t>
         </is>
       </c>
     </row>
@@ -2272,22 +2272,22 @@
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
-          <t>Optimizing the NMR workflow for protein dynamics experiments</t>
+          <t>OPTIMIZING THE NMR WORKFLOW FOR PROTEIN DYNAMICS EXPERIMENTS</t>
         </is>
       </c>
       <c r="C47" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D47" s="0" t="inlineStr">
         <is>
-          <t>Clemens Anklin</t>
+          <t>CLEMENS ANKLIN</t>
         </is>
       </c>
       <c r="E47" s="0" t="inlineStr">
         <is>
-          <t>Bruker</t>
+          <t>BRUKER</t>
         </is>
       </c>
     </row>
@@ -2297,42 +2297,42 @@
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
-          <t>THE FAT BLOOD: QUANTIFICATION OF BLOOD PLASMA METABOLITES AND LIPOPROTEINS FROM 1H NMR SPECTRA USING SIGNATURE MAPPING (SigMa) APPROACH</t>
+          <t>THE FAT BLOOD: QUANTIFICATION OF BLOOD PLASMA METABOLITES AND LIPOPROTEINS FROM 1H NMR SPECTRA USING SIGNATURE MAPPING (SIGMA) APPROACH</t>
         </is>
       </c>
       <c r="C48" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D48" s="0" t="inlineStr">
         <is>
-          <t>Søren Balling Engelsen</t>
+          <t>SØREN BALLING ENGELSEN</t>
         </is>
       </c>
       <c r="E48" s="0" t="inlineStr">
         <is>
-          <t>University of Copenhagen</t>
+          <t>UNIVERSITY OF COPENHAGEN</t>
         </is>
       </c>
       <c r="F48" s="0" t="inlineStr">
         <is>
-          <t> Bekzod  Khakimov </t>
+          <t> BEKZOD  KHAKIMOV </t>
         </is>
       </c>
       <c r="G48" s="0" t="inlineStr">
         <is>
-          <t>University of Copenhagen</t>
+          <t>UNIVERSITY OF COPENHAGEN</t>
         </is>
       </c>
       <c r="H48" s="0" t="inlineStr">
         <is>
-          <t> Viola  Aru</t>
+          <t> VIOLA  ARU</t>
         </is>
       </c>
       <c r="I48" s="0" t="inlineStr">
         <is>
-          <t>University of Copenhagen</t>
+          <t>UNIVERSITY OF COPENHAGEN</t>
         </is>
       </c>
     </row>
@@ -2342,22 +2342,22 @@
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
-          <t>Hélio - Uma visão geral do mercado</t>
+          <t>HÉLIO - UMA VISÃO GERAL DO MERCADO</t>
         </is>
       </c>
       <c r="C49" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D49" s="0" t="inlineStr">
         <is>
-          <t>Felipe Simoes</t>
+          <t>FELIPE SIMOES</t>
         </is>
       </c>
       <c r="E49" s="0" t="inlineStr">
         <is>
-          <t>Hélio para Ressonancia Magnética / Hélio para Ressonancia Magnética / Air Products do Brasil Ltda</t>
+          <t>HÉLIO PARA RESSONANCIA MAGNÉTICA / HÉLIO PARA RESSONANCIA MAGNÉTICA / AIR PRODUCTS DO BRASIL LTDA</t>
         </is>
       </c>
     </row>
@@ -2372,17 +2372,17 @@
       </c>
       <c r="C50" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D50" s="0" t="inlineStr">
         <is>
-          <t>Marcel Lachenmann</t>
+          <t>MARCEL LACHENMANN</t>
         </is>
       </c>
       <c r="E50" s="0" t="inlineStr">
         <is>
-          <t>Oxford Instruments</t>
+          <t>OXFORD INSTRUMENTS</t>
         </is>
       </c>
     </row>
@@ -2397,17 +2397,17 @@
       </c>
       <c r="C51" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D51" s="0" t="inlineStr">
         <is>
-          <t>Hector Robert</t>
+          <t>HECTOR ROBERT</t>
         </is>
       </c>
       <c r="E51" s="0" t="inlineStr">
         <is>
-          <t>Magritek, Inc</t>
+          <t>MAGRITEK, INC</t>
         </is>
       </c>
     </row>
@@ -2422,17 +2422,17 @@
       </c>
       <c r="C52" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D52" s="0" t="inlineStr">
         <is>
-          <t>Marcus Vinícius Cangussu Cardoso</t>
+          <t>MARCUS VINÍCIUS CANGUSSU CARDOSO</t>
         </is>
       </c>
       <c r="E52" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de Ouro Preto</t>
+          <t>UNIVERSIDADE FEDERAL DE OURO PRETO</t>
         </is>
       </c>
     </row>
@@ -2447,17 +2447,17 @@
       </c>
       <c r="C53" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D53" s="0" t="inlineStr">
         <is>
-          <t>Annick Moing</t>
+          <t>ANNICK MOING</t>
         </is>
       </c>
       <c r="E53" s="0" t="inlineStr">
         <is>
-          <t>INRAE Bordeaux, France</t>
+          <t>INRAE BORDEAUX, FRANCE</t>
         </is>
       </c>
     </row>
@@ -2467,62 +2467,62 @@
       </c>
       <c r="B54" s="0" t="inlineStr">
         <is>
-          <t>Solid-state NMR investigation of Na5RESi4O12-based (RE = Sc, Y) glass-ceramics</t>
+          <t>SOLID-STATE NMR INVESTIGATION OF NA5RESI4O12-BASED (RE = SC, Y) GLASS-CERAMICS</t>
         </is>
       </c>
       <c r="C54" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D54" s="0" t="inlineStr">
         <is>
-          <t>Igor d'Anciães Almeida Silva</t>
+          <t>IGOR D'ANCIÃES ALMEIDA SILVA</t>
         </is>
       </c>
       <c r="E54" s="0" t="inlineStr">
         <is>
-          <t>Universidade de São Paulo</t>
+          <t>UNIVERSIDADE DE SÃO PAULO</t>
         </is>
       </c>
       <c r="F54" s="0" t="inlineStr">
         <is>
-          <t> Hellmut Eckert</t>
+          <t> HELLMUT ECKERT</t>
         </is>
       </c>
       <c r="G54" s="0" t="inlineStr">
         <is>
-          <t>Universidade de São Paulo</t>
+          <t>UNIVERSIDADE DE SÃO PAULO</t>
         </is>
       </c>
       <c r="H54" s="0" t="inlineStr">
         <is>
-          <t> Ana Candida Martins Rodrigues</t>
+          <t> ANA CANDIDA MARTINS RODRIGUES</t>
         </is>
       </c>
       <c r="I54" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de São Carlos</t>
+          <t>UNIVERSIDADE FEDERAL DE SÃO CARLOS</t>
         </is>
       </c>
       <c r="J54" s="0" t="inlineStr">
         <is>
-          <t> Adraiana Nieto-Munoz</t>
+          <t> ADRAIANA NIETO-MUNOZ</t>
         </is>
       </c>
       <c r="K54" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de São Carlos</t>
+          <t>UNIVERSIDADE FEDERAL DE SÃO CARLOS</t>
         </is>
       </c>
       <c r="L54" s="0" t="inlineStr">
         <is>
-          <t> Vinicius Zallocco</t>
+          <t> VINICIUS ZALLOCCO</t>
         </is>
       </c>
       <c r="M54" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal de São Carlos</t>
+          <t>UNIVERSIDADE FEDERAL DE SÃO CARLOS</t>
         </is>
       </c>
     </row>
@@ -2532,22 +2532,22 @@
       </c>
       <c r="B55" s="0" t="inlineStr">
         <is>
-          <t>Fast field-cycling NMR Relaxometry: methodology and applications</t>
+          <t>FAST FIELD-CYCLING NMR RELAXOMETRY: METHODOLOGY AND APPLICATIONS</t>
         </is>
       </c>
       <c r="C55" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D55" s="0" t="inlineStr">
         <is>
-          <t>Esteban Anoardo</t>
+          <t>ESTEBAN ANOARDO</t>
         </is>
       </c>
       <c r="E55" s="0" t="inlineStr">
         <is>
-          <t>Laboratorio de Relaxometría y Técnicas Especiales (LaRTE). / Instituto de Física Enrique Gaviola, CONICET. Córdoba, Argentina. / FaMAF - Universidad Nacional de Córdoba. Córdoba, Argentina.</t>
+          <t>LABORATORIO DE RELAXOMETRÍA Y TÉCNICAS ESPECIALES (LARTE). / INSTITUTO DE FÍSICA ENRIQUE GAVIOLA, CONICET. CÓRDOBA, ARGENTINA. / FAMAF - UNIVERSIDAD NACIONAL DE CÓRDOBA. CÓRDOBA, ARGENTINA.</t>
         </is>
       </c>
     </row>
@@ -2562,187 +2562,187 @@
       </c>
       <c r="C56" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D56" s="0" t="inlineStr">
         <is>
-          <t>Amy Jenne</t>
+          <t>AMY JENNE</t>
         </is>
       </c>
       <c r="E56" s="0" t="inlineStr">
         <is>
-          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+          <t>CHEMISTRY / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="F56" s="0" t="inlineStr">
         <is>
-          <t> Sebastian Von Der Ecken</t>
+          <t> SEBASTIAN VON DER ECKEN</t>
         </is>
       </c>
       <c r="G56" s="0" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="H56" s="0" t="inlineStr">
         <is>
-          <t> Vincent Moxley-Paquette</t>
+          <t> VINCENT MOXLEY-PAQUETTE</t>
         </is>
       </c>
       <c r="I56" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="J56" s="0" t="inlineStr">
         <is>
-          <t> Ian Swyer</t>
+          <t> IAN SWYER</t>
         </is>
       </c>
       <c r="K56" s="0" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="L56" s="0" t="inlineStr">
         <is>
-          <t> Ronald Soong</t>
+          <t> RONALD SOONG</t>
         </is>
       </c>
       <c r="M56" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="N56" s="0" t="inlineStr">
         <is>
-          <t> Monica Bastawrous</t>
+          <t> MONICA BASTAWROUS</t>
         </is>
       </c>
       <c r="O56" s="0" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="P56" s="0" t="inlineStr">
         <is>
-          <t> Falko Busse</t>
+          <t> FALKO BUSSE</t>
         </is>
       </c>
       <c r="Q56" s="0" t="inlineStr">
         <is>
-          <t>Bruker</t>
+          <t>BRUKER</t>
         </is>
       </c>
       <c r="R56" s="0" t="inlineStr">
         <is>
-          <t> Wolfgang Bermel</t>
+          <t> WOLFGANG BERMEL</t>
         </is>
       </c>
       <c r="S56" s="0" t="inlineStr">
         <is>
-          <t>Biospin GmbH / BRUKER</t>
+          <t>BIOSPIN GMBH / BRUKER</t>
         </is>
       </c>
       <c r="T56" s="0" t="inlineStr">
         <is>
-          <t> Daniel Schmidig</t>
+          <t> DANIEL SCHMIDIG</t>
         </is>
       </c>
       <c r="U56" s="0" t="inlineStr">
         <is>
-          <t>Biospin AG / BRUKER</t>
+          <t>BIOSPIN AG / BRUKER</t>
         </is>
       </c>
       <c r="V56" s="0" t="inlineStr">
         <is>
-          <t> Till Kuehn</t>
+          <t> TILL KUEHN</t>
         </is>
       </c>
       <c r="W56" s="0" t="inlineStr">
         <is>
-          <t>Biospin AG / BRUKER</t>
+          <t>BIOSPIN AG / BRUKER</t>
         </is>
       </c>
       <c r="X56" s="0" t="inlineStr">
         <is>
-          <t> Rainer Kuemmerle</t>
+          <t> RAINER KUEMMERLE</t>
         </is>
       </c>
       <c r="Y56" s="0" t="inlineStr">
         <is>
-          <t>Biospin AG / BRUKER</t>
+          <t>BIOSPIN AG / BRUKER</t>
         </is>
       </c>
       <c r="Z56" s="0" t="inlineStr">
         <is>
-          <t> Danijela Al Adwan-Stojilkovic</t>
+          <t> DANIJELA AL ADWAN-STOJILKOVIC</t>
         </is>
       </c>
       <c r="AA56" s="0" t="inlineStr">
         <is>
-          <t>Biospin AG / BRUKER</t>
+          <t>BIOSPIN AG / BRUKER</t>
         </is>
       </c>
       <c r="AB56" s="0" t="inlineStr">
         <is>
-          <t> Stephan Graf</t>
+          <t> STEPHAN GRAF</t>
         </is>
       </c>
       <c r="AC56" s="0" t="inlineStr">
         <is>
-          <t>Biospin AG / BRUKER</t>
+          <t>BIOSPIN AG / BRUKER</t>
         </is>
       </c>
       <c r="AD56" s="0" t="inlineStr">
         <is>
-          <t> Thomas Frei</t>
+          <t> THOMAS FREI</t>
         </is>
       </c>
       <c r="AE56" s="0" t="inlineStr">
         <is>
-          <t>Biospin AG / BRUKER</t>
+          <t>BIOSPIN AG / BRUKER</t>
         </is>
       </c>
       <c r="AF56" s="0" t="inlineStr">
         <is>
-          <t> Martine Monette</t>
+          <t> MARTINE MONETTE</t>
         </is>
       </c>
       <c r="AG56" s="0" t="inlineStr">
         <is>
-          <t>Canada Ltd / BRUKER</t>
+          <t>CANADA LTD / BRUKER</t>
         </is>
       </c>
       <c r="AH56" s="0" t="inlineStr">
         <is>
-          <t> Henry Stronks</t>
+          <t> HENRY STRONKS</t>
         </is>
       </c>
       <c r="AI56" s="0" t="inlineStr">
         <is>
-          <t>Canada Ltd / BRUKER</t>
+          <t>CANADA LTD / BRUKER</t>
         </is>
       </c>
       <c r="AJ56" s="0" t="inlineStr">
         <is>
-          <t> Aaron Wheeler</t>
+          <t> AARON WHEELER</t>
         </is>
       </c>
       <c r="AK56" s="0" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="AL56" s="0" t="inlineStr">
         <is>
-          <t> Andre Simpson</t>
+          <t> ANDRE SIMPSON</t>
         </is>
       </c>
       <c r="AM56" s="0" t="inlineStr">
         <is>
-          <t>University of Toronto</t>
+          <t>UNIVERSITY OF TORONTO</t>
         </is>
       </c>
     </row>
@@ -2752,142 +2752,142 @@
       </c>
       <c r="B57" s="0" t="inlineStr">
         <is>
-          <t>Investigating inverse and direct 13C detect experiments and slow spinning of in vivo multiphase samples</t>
+          <t>INVESTIGATING INVERSE AND DIRECT 13C DETECT EXPERIMENTS AND SLOW SPINNING OF IN VIVO MULTIPHASE SAMPLES</t>
         </is>
       </c>
       <c r="C57" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D57" s="0" t="inlineStr">
         <is>
-          <t>Rajshree Ghosh Biswas</t>
+          <t>RAJSHREE GHOSH BISWAS</t>
         </is>
       </c>
       <c r="E57" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="F57" s="0" t="inlineStr">
         <is>
-          <t> Ronald Soong</t>
+          <t> RONALD SOONG</t>
         </is>
       </c>
       <c r="G57" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="H57" s="0" t="inlineStr">
         <is>
-          <t> Paris Ning</t>
+          <t> PARIS NING</t>
         </is>
       </c>
       <c r="I57" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="J57" s="0" t="inlineStr">
         <is>
-          <t> Daniel Lane</t>
+          <t> DANIEL LANE</t>
         </is>
       </c>
       <c r="K57" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="L57" s="0" t="inlineStr">
         <is>
-          <t> Daniel Schmidig</t>
+          <t> DANIEL SCHMIDIG</t>
         </is>
       </c>
       <c r="M57" s="0" t="inlineStr">
         <is>
-          <t>Biospin AG / Bruker</t>
+          <t>BIOSPIN AG / BRUKER</t>
         </is>
       </c>
       <c r="N57" s="0" t="inlineStr">
         <is>
-          <t> Peter de Castro</t>
+          <t> PETER DE CASTRO</t>
         </is>
       </c>
       <c r="O57" s="0" t="inlineStr">
         <is>
-          <t>Biospin AG / Bruker</t>
+          <t>BIOSPIN AG / BRUKER</t>
         </is>
       </c>
       <c r="P57" s="0" t="inlineStr">
         <is>
-          <t> Stephan Graf</t>
+          <t> STEPHAN GRAF</t>
         </is>
       </c>
       <c r="Q57" s="0" t="inlineStr">
         <is>
-          <t>Biospin AG / Bruker</t>
+          <t>BIOSPIN AG / BRUKER</t>
         </is>
       </c>
       <c r="R57" s="0" t="inlineStr">
         <is>
-          <t> Sebastian Wegner</t>
+          <t> SEBASTIAN WEGNER</t>
         </is>
       </c>
       <c r="S57" s="0" t="inlineStr">
         <is>
-          <t>Bruker Biospin GmbH / Bruker</t>
+          <t>BRUKER BIOSPIN GMBH / BRUKER</t>
         </is>
       </c>
       <c r="T57" s="0" t="inlineStr">
         <is>
-          <t> Falko Busse</t>
+          <t> FALKO BUSSE</t>
         </is>
       </c>
       <c r="U57" s="0" t="inlineStr">
         <is>
-          <t>Bruker Biospin GmbH / Bruker</t>
+          <t>BRUKER BIOSPIN GMBH / BRUKER</t>
         </is>
       </c>
       <c r="V57" s="0" t="inlineStr">
         <is>
-          <t> Jochem Struppe</t>
+          <t> JOCHEM STRUPPE</t>
         </is>
       </c>
       <c r="W57" s="0" t="inlineStr">
         <is>
-          <t>Bruker BioSpin</t>
+          <t>BRUKER BIOSPIN</t>
         </is>
       </c>
       <c r="X57" s="0" t="inlineStr">
         <is>
-          <t> Michael  Fey</t>
+          <t> MICHAEL  FEY</t>
         </is>
       </c>
       <c r="Y57" s="0" t="inlineStr">
         <is>
-          <t>Bruker</t>
+          <t>BRUKER</t>
         </is>
       </c>
       <c r="Z57" s="0" t="inlineStr">
         <is>
-          <t> Myrna Simpson</t>
+          <t> MYRNA SIMPSON</t>
         </is>
       </c>
       <c r="AA57" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
       <c r="AB57" s="0" t="inlineStr">
         <is>
-          <t> Andre Simpson</t>
+          <t> ANDRE SIMPSON</t>
         </is>
       </c>
       <c r="AC57" s="0" t="inlineStr">
         <is>
-          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+          <t>DEPARTMENT OF PHYSICAL AND ENVIRONMENTAL SCIENCE / SCARBOROUGH CAMPUS / UNIVERSITY OF TORONTO</t>
         </is>
       </c>
     </row>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="C58" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D58" s="0" t="inlineStr">
@@ -2912,57 +2912,57 @@
       </c>
       <c r="E58" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Estado do Rio de Janeiro</t>
+          <t>UNIVERSIDADE FEDERAL DO ESTADO DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="F58" s="0" t="inlineStr">
         <is>
-          <t> Talita Stelling De Araujo</t>
+          <t> TALITA STELLING DE ARAUJO</t>
         </is>
       </c>
       <c r="G58" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Rio de Janeiro</t>
+          <t>UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="H58" s="0" t="inlineStr">
         <is>
-          <t> Rafael Alves de Andrade</t>
+          <t> RAFAEL ALVES DE ANDRADE</t>
         </is>
       </c>
       <c r="I58" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Rio de Janeiro</t>
+          <t>UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="J58" s="0" t="inlineStr">
         <is>
-          <t> Fabio C. L. Almeida</t>
+          <t> FABIO C. L. ALMEIDA</t>
         </is>
       </c>
       <c r="K58" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Rio de Janeiro</t>
+          <t>UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="L58" s="0" t="inlineStr">
         <is>
-          <t> Marcius da Silva Almeida</t>
+          <t> MARCIUS DA SILVA ALMEIDA</t>
         </is>
       </c>
       <c r="M58" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Rio de Janeiro</t>
+          <t>UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
       <c r="N58" s="0" t="inlineStr">
         <is>
-          <t> Claudia Jorge do Nascimento</t>
+          <t> CLAUDIA JORGE DO NASCIMENTO</t>
         </is>
       </c>
       <c r="O58" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Estado do Rio de Janeiro</t>
+          <t>UNIVERSIDADE FEDERAL DO ESTADO DO RIO DE JANEIRO</t>
         </is>
       </c>
     </row>
@@ -2977,17 +2977,17 @@
       </c>
       <c r="C59" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D59" s="0" t="inlineStr">
         <is>
-          <t>Fabio Ceneviva  Lacerda Almeida</t>
+          <t>FABIO CENEVIVA  LACERDA ALMEIDA</t>
         </is>
       </c>
       <c r="E59" s="0" t="inlineStr">
         <is>
-          <t>Universidade Federal do Rio de Janeiro</t>
+          <t>UNIVERSIDADE FEDERAL DO RIO DE JANEIRO</t>
         </is>
       </c>
     </row>
@@ -3002,17 +3002,17 @@
       </c>
       <c r="C60" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D60" s="0" t="inlineStr">
         <is>
-          <t>Clemens  Anklin</t>
+          <t>CLEMENS  ANKLIN</t>
         </is>
       </c>
       <c r="E60" s="0" t="inlineStr">
         <is>
-          <t>NMR Applicaitons / Bruker Biospin</t>
+          <t>NMR APPLICAITONS / BRUKER BIOSPIN</t>
         </is>
       </c>
     </row>
@@ -3022,22 +3022,22 @@
       </c>
       <c r="B61" s="0" t="inlineStr">
         <is>
-          <t>Lead Generation without an X-Ray Crystal Structure: An NMR Method to Probe Protein-Ligand Complexes</t>
+          <t>LEAD GENERATION WITHOUT AN X-RAY CRYSTAL STRUCTURE: AN NMR METHOD TO PROBE PROTEIN-LIGAND COMPLEXES</t>
         </is>
       </c>
       <c r="C61" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D61" s="0" t="inlineStr">
         <is>
-          <t>Julien Orts</t>
+          <t>JULIEN ORTS</t>
         </is>
       </c>
       <c r="E61" s="0" t="inlineStr">
         <is>
-          <t>Department of Pharmaceutical Sciences / Faculty of Life Sciences / University of Vienna</t>
+          <t>DEPARTMENT OF PHARMACEUTICAL SCIENCES / FACULTY OF LIFE SCIENCES / UNIVERSITY OF VIENNA</t>
         </is>
       </c>
     </row>
@@ -3047,22 +3047,22 @@
       </c>
       <c r="B62" s="0" t="inlineStr">
         <is>
-          <t>Q.One NMR A New Dimension in NMR</t>
+          <t>Q.ONE NMR A NEW DIMENSION IN NMR</t>
         </is>
       </c>
       <c r="C62" s="0" t="inlineStr">
         <is>
-          <t>Invited Lecturer</t>
+          <t>INVITED LECTURER</t>
         </is>
       </c>
       <c r="D62" s="0" t="inlineStr">
         <is>
-          <t>Donald Bouchard</t>
+          <t>DONALD BOUCHARD</t>
         </is>
       </c>
       <c r="E62" s="0" t="inlineStr">
         <is>
-          <t>Alegre Science Inc</t>
+          <t>ALEGRE SCIENCE INC</t>
         </is>
       </c>
     </row>
@@ -3077,57 +3077,57 @@
       </c>
       <c r="C63" s="0" t="inlineStr">
         <is>
-          <t>Poster Presentation</t>
+          <t>POSTER PRESENTATION</t>
         </is>
       </c>
       <c r="D63" s="0" t="inlineStr">
         <is>
-          <t>Giselle de Araujo Lima e Souza</t>
+          <t>GISELLE DE ARAUJO LIMA E SOUZA</t>
         </is>
       </c>
       <c r="E63" s="0" t="inlineStr">
         <is>
-          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
+          <t>DEPARTMENT OF CHEMISTRY, MATERIALS AND CHEMICAL ENGINEERING “GIULIO NATTA” / POLITECNICO DI MILANO</t>
         </is>
       </c>
       <c r="F63" s="0" t="inlineStr">
         <is>
-          <t> Maria Enrica Di Pietro</t>
+          <t> MARIA ENRICA DI PIETRO</t>
         </is>
       </c>
       <c r="G63" s="0" t="inlineStr">
         <is>
-          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
+          <t>DEPARTMENT OF CHEMISTRY, MATERIALS AND CHEMICAL ENGINEERING “GIULIO NATTA” / POLITECNICO DI MILANO</t>
         </is>
       </c>
       <c r="H63" s="0" t="inlineStr">
         <is>
-          <t> Giovanni Battista Appetecchi</t>
+          <t> GIOVANNI BATTISTA APPETECCHI</t>
         </is>
       </c>
       <c r="I63" s="0" t="inlineStr">
         <is>
-          <t>Department for Sustainability (SSPT) / Italian National Agency for New Technologies, Energy and Sustainable Economic Development / ENEA</t>
+          <t>DEPARTMENT FOR SUSTAINABILITY (SSPT) / ITALIAN NATIONAL AGENCY FOR NEW TECHNOLOGIES, ENERGY AND SUSTAINABLE ECONOMIC DEVELOPMENT / ENEA</t>
         </is>
       </c>
       <c r="J63" s="0" t="inlineStr">
         <is>
-          <t> Patricia Fazzio Martinez</t>
+          <t> PATRICIA FAZZIO MARTINEZ</t>
         </is>
       </c>
       <c r="K63" s="0" t="inlineStr">
         <is>
-          <t>School of Chemical Engineering/ University of Campinas/ Campinas/ Brazil</t>
+          <t>SCHOOL OF CHEMICAL ENGINEERING/ UNIVERSITY OF CAMPINAS/ CAMPINAS/ BRAZIL</t>
         </is>
       </c>
       <c r="L63" s="0" t="inlineStr">
         <is>
-          <t> Andrea Mele</t>
+          <t> ANDREA MELE</t>
         </is>
       </c>
       <c r="M63" s="0" t="inlineStr">
         <is>
-          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
+          <t>DEPARTMENT OF CHEMISTRY, MATERIALS AND CHEMICAL ENGINEERING “GIULIO NATTA” / POLITECNICO DI MILANO</t>
         </is>
       </c>
     </row>

</xml_diff>